<commit_message>
DivisionTerritoriale : préciser les types attendus pour les offres et les EG (#458)
* DivisionTerritoriale : préciser les types attendus pour les offres et les EG

* Update RORHealthcareService.fsh

* Update ROROrganization.fsh

* contrainte sortie de la description 5dae12a1699afda677ccf5daf1efdb4251bc9157
</commit_message>
<xml_diff>
--- a/sg/mappingFHIR-ROR/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/sg/mappingFHIR-ROR/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-26T14:22:26+00:00</t>
+    <t>2026-01-26T14:31:20+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -794,7 +794,7 @@
 </t>
   </si>
   <si>
-    <t>uniteSensible (OffreOperationnelle) : Permet de signaler que toutes les informations de description d'une offre sont confidentielles ou que le porteur d'offre ne souhaite pas diffuser</t>
+    <t>uniteSensible (OffreOperationnelle) : Permet de signaler que toutes les informations de description d'une offre sont confidentielles</t>
   </si>
   <si>
     <t>Extension créée dans le cadre du ROR pour signaler que toutes les informations de description d'une offre sont confidentielles car elles présentent un risque d'utilisation à des fins malveillantes, ou que le porteur d'offre ne souhaite pas diffuser.</t>

</xml_diff>